<commit_message>
need to change the instruction set in the excel file and need to give new instruction for stack adresssing push and pop which are have been put in the cpu but not in control unit
</commit_message>
<xml_diff>
--- a/Instruction Set.xlsx
+++ b/Instruction Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Logisim Evolution\simulations\CP-V0-08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157A17A-5563-49E9-83E9-2FD919A4721A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CAF2CD-FCB2-4358-B10C-07EEDA1B4DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1633FD8-4BD1-42FD-B44A-C491D056B199}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="146">
   <si>
     <t>ALU</t>
   </si>
@@ -216,27 +216,6 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>100XX000</t>
-  </si>
-  <si>
-    <t>100XX001</t>
-  </si>
-  <si>
-    <t>100XX010</t>
-  </si>
-  <si>
-    <t>100XX011</t>
-  </si>
-  <si>
-    <t>100XX100</t>
-  </si>
-  <si>
-    <t>100XX101</t>
-  </si>
-  <si>
-    <t>100XX110</t>
-  </si>
-  <si>
     <t>ADDI</t>
   </si>
   <si>
@@ -297,9 +276,6 @@
     <t>001 XX 100</t>
   </si>
   <si>
-    <t>010 11 RX</t>
-  </si>
-  <si>
     <t>010 10 RX</t>
   </si>
   <si>
@@ -309,21 +285,9 @@
     <t>010 11 001</t>
   </si>
   <si>
-    <t>MOVE/PUSH          RX, RAM</t>
-  </si>
-  <si>
     <t>MOVE                     ACC,A/Rx</t>
   </si>
   <si>
-    <t>POP                         RAM to A/R0</t>
-  </si>
-  <si>
-    <t>PUSH                       ACC to RAM</t>
-  </si>
-  <si>
-    <t>LD                            RAM to Rx</t>
-  </si>
-  <si>
     <t>STORE                     ACC to RAM Addr</t>
   </si>
   <si>
@@ -340,6 +304,174 @@
   </si>
   <si>
     <t>011XX111</t>
+  </si>
+  <si>
+    <t>100X0110</t>
+  </si>
+  <si>
+    <t>100X0101</t>
+  </si>
+  <si>
+    <t>100X0100</t>
+  </si>
+  <si>
+    <t>100X0011</t>
+  </si>
+  <si>
+    <t>100X0010</t>
+  </si>
+  <si>
+    <t>100X0001</t>
+  </si>
+  <si>
+    <t>100X0000</t>
+  </si>
+  <si>
+    <t>100X1000</t>
+  </si>
+  <si>
+    <t>Decrement / Increment</t>
+  </si>
+  <si>
+    <t>LOAD the current PC to Temp Inst</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>check for zero</t>
+  </si>
+  <si>
+    <t>IF (Zero):</t>
+  </si>
+  <si>
+    <t>ELSE:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Coutine to the next instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        RET: 011XX111</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>4X</t>
+  </si>
+  <si>
+    <t>5X</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>POP                         Stack to Rx</t>
+  </si>
+  <si>
+    <t>PUSH                       Rx to Stack</t>
+  </si>
+  <si>
+    <t>LOAD                      RAM to Rx</t>
+  </si>
+  <si>
+    <t>Move/RAM             ACC to RAM</t>
+  </si>
+  <si>
+    <t>010 11 010</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
   </si>
 </sst>
 </file>
@@ -722,22 +854,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D464CC2-A764-4AA8-92F7-D3D9EBE0103F}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.21875" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -748,7 +881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -759,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -770,7 +903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -781,7 +914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -792,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -803,7 +936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -814,7 +947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -825,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -836,87 +969,111 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>67</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>68</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>70</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>71</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>72</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>73</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>74</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
@@ -924,45 +1081,60 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>75</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="C24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>76</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="C25" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>77</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="C26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>78</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="C27" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>79</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
@@ -970,63 +1142,81 @@
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>65</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="C34" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>66</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="C35" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="C36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>80</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="C37" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1"/>
-    <row r="43" spans="1:5">
+        <v>81</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1"/>
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
         <v>38</v>
       </c>
@@ -1034,72 +1224,96 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="C44" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="C45" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="E45" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="C46" t="s">
         <v>40</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="E46" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="C47" t="s">
         <v>41</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="E47" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="C48" t="s">
         <v>42</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="E48" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="C49" t="s">
         <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>88</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="C50" t="s">
         <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
@@ -1110,64 +1324,144 @@
         <v>53</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>96</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="C54" t="s">
         <v>54</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>95</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="C55" t="s">
         <v>55</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>94</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="C56" t="s">
         <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>93</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="C57" t="s">
         <v>57</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>92</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="C58" t="s">
         <v>58</v>
       </c>
       <c r="D58" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>91</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="C59" t="s">
         <v>59</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
-      </c>
-      <c r="E59" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" t="s">
         <v>97</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="B68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="B69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="B71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="B72" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="B73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="B74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="B75" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add docs folder containing images of the project
</commit_message>
<xml_diff>
--- a/Instruction Set.xlsx
+++ b/Instruction Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Logisim Evolution\simulations\CP-V0-08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CAF2CD-FCB2-4358-B10C-07EEDA1B4DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C360E-8E16-41D4-92CC-2FD96EC834C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1633FD8-4BD1-42FD-B44A-C491D056B199}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
   <si>
     <t>ALU</t>
   </si>
@@ -138,24 +138,12 @@
     <t>111</t>
   </si>
   <si>
-    <t>001XX</t>
-  </si>
-  <si>
-    <t>000XX</t>
-  </si>
-  <si>
     <t>MEM</t>
   </si>
   <si>
-    <t>010XX</t>
-  </si>
-  <si>
     <t>BRANCH</t>
   </si>
   <si>
-    <t>011XX</t>
-  </si>
-  <si>
     <t>JZ</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>OTHERS</t>
   </si>
   <si>
-    <t>100XX</t>
-  </si>
-  <si>
     <t>CMP</t>
   </si>
   <si>
@@ -231,60 +216,9 @@
     <t>MOVI</t>
   </si>
   <si>
-    <t>010 00 RX</t>
-  </si>
-  <si>
     <t>010 01 RX</t>
   </si>
   <si>
-    <t>000 XX 111</t>
-  </si>
-  <si>
-    <t>000 XX 110</t>
-  </si>
-  <si>
-    <t>000 XX 101</t>
-  </si>
-  <si>
-    <t>000 XX 100</t>
-  </si>
-  <si>
-    <t>000 XX 011</t>
-  </si>
-  <si>
-    <t>000 XX 010</t>
-  </si>
-  <si>
-    <t>000 XX 001</t>
-  </si>
-  <si>
-    <t>000 XX 000</t>
-  </si>
-  <si>
-    <t>001 XX 000</t>
-  </si>
-  <si>
-    <t>001 XX 001</t>
-  </si>
-  <si>
-    <t>001 XX 010</t>
-  </si>
-  <si>
-    <t>001 XX 011</t>
-  </si>
-  <si>
-    <t>001 XX 100</t>
-  </si>
-  <si>
-    <t>010 10 RX</t>
-  </si>
-  <si>
-    <t>010 11 000</t>
-  </si>
-  <si>
-    <t>010 11 001</t>
-  </si>
-  <si>
     <t>MOVE                     ACC,A/Rx</t>
   </si>
   <si>
@@ -396,12 +330,6 @@
     <t>24</t>
   </si>
   <si>
-    <t>4X</t>
-  </si>
-  <si>
-    <t>5X</t>
-  </si>
-  <si>
     <t>61</t>
   </si>
   <si>
@@ -462,23 +390,83 @@
     <t>Move/RAM             ACC to RAM</t>
   </si>
   <si>
-    <t>010 11 010</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
+    <t>STACK</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>000 00 111</t>
+  </si>
+  <si>
+    <t>000 00 110</t>
+  </si>
+  <si>
+    <t>000 00 101</t>
+  </si>
+  <si>
+    <t>000 00 100</t>
+  </si>
+  <si>
+    <t>000 00 011</t>
+  </si>
+  <si>
+    <t>000 00 010</t>
+  </si>
+  <si>
+    <t>000 00 001</t>
+  </si>
+  <si>
+    <t>000 00 000</t>
+  </si>
+  <si>
+    <t>000 10 000</t>
+  </si>
+  <si>
+    <t>000 10 001</t>
+  </si>
+  <si>
+    <t>000 10 010</t>
+  </si>
+  <si>
+    <t>000 10 011</t>
+  </si>
+  <si>
+    <t>000 10 100</t>
+  </si>
+  <si>
+    <t>001-010</t>
+  </si>
+  <si>
+    <t>001 01 RX</t>
+  </si>
+  <si>
+    <t>001 10 RX</t>
+  </si>
+  <si>
+    <t>001 11 RX</t>
+  </si>
+  <si>
+    <t>001 00 RX</t>
+  </si>
+  <si>
+    <t>2X</t>
+  </si>
+  <si>
+    <t>3X</t>
+  </si>
+  <si>
+    <t>010 00 001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,8 +487,15 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +506,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -526,12 +527,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -540,6 +538,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,25 +859,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D464CC2-A764-4AA8-92F7-D3D9EBE0103F}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.21875" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="8.88671875" style="3"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -882,10 +885,10 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -893,10 +896,10 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -904,10 +907,10 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -915,10 +918,10 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -926,10 +929,10 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -937,10 +940,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -948,10 +951,10 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -959,23 +962,23 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>85</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -983,13 +986,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>85</v>
+        <v>122</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -997,13 +1000,13 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>85</v>
+        <v>123</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1011,13 +1014,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>85</v>
+        <v>124</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1025,13 +1028,13 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>85</v>
+        <v>125</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1039,13 +1042,13 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>85</v>
+        <v>126</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1053,13 +1056,13 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>85</v>
+        <v>127</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1067,401 +1070,418 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>114</v>
+        <v>128</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
-        <v>34</v>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>115</v>
+        <v>129</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="C24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="C25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>117</v>
+        <v>131</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="C26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>118</v>
+        <v>132</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1">
+      <c r="C40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="7">
+        <v>50</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
         <v>64</v>
       </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="C34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="C35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="C37" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="C38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="C39" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1"/>
-    <row r="43" spans="1:6">
-      <c r="A43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="C44" t="s">
-        <v>87</v>
-      </c>
       <c r="D44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>122</v>
+        <v>41</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="C45" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>124</v>
+        <v>42</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="C46" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="C47" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>126</v>
+        <v>44</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="C48" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>127</v>
+        <v>45</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="C49" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>128</v>
+        <v>46</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="C50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>130</v>
+        <v>66</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:6">
+      <c r="A54" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>131</v>
+        <v>74</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="C55" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D55" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>132</v>
+        <v>73</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="C56" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>133</v>
+        <v>72</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="C57" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>92</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="C58" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>85</v>
+        <v>70</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="C59" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>85</v>
+        <v>69</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="C60" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>137</v>
+        <v>68</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
+        <v>75</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B67" t="s">
-        <v>99</v>
+      <c r="A67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="B68" t="s">
-        <v>100</v>
+      <c r="B68" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="B69" t="s">
-        <v>101</v>
+      <c r="B69" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="B70" t="s">
-        <v>101</v>
+      <c r="B70" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="B71" t="s">
-        <v>102</v>
+      <c r="B71" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="B72" t="s">
-        <v>103</v>
+      <c r="B72" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="B73" t="s">
-        <v>105</v>
+      <c r="B73" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="B74" t="s">
-        <v>104</v>
+      <c r="B74" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="B75" t="s">
-        <v>106</v>
+      <c r="B75" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>